<commit_message>
updated testing of ValidLogin and InValidLogin
</commit_message>
<xml_diff>
--- a/Dolibar/data/input.xlsx
+++ b/Dolibar/data/input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -27,13 +27,22 @@
     <t>HomePageTittle</t>
   </si>
   <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
     <t>manager</t>
   </si>
   <si>
-    <t>Enter</t>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -69,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -384,7 +394,7 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,16 +404,29 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>